<commit_message>
adding logo and normalisation
</commit_message>
<xml_diff>
--- a/Data_Dictonary.xlsx
+++ b/Data_Dictonary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Monolith\Desktop\Projects\INFT-3050-web-programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8463245-23B8-401C-B88C-7F72CD1AE5A0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83787620-F551-4086-8E2D-E8A064EF2846}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{BCA443CA-9BD8-47A8-B013-DA655F05E55C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="84">
   <si>
     <t>Customer</t>
   </si>
@@ -271,6 +271,12 @@
   </si>
   <si>
     <t>VarChar(3000)</t>
+  </si>
+  <si>
+    <t>lastEdited</t>
+  </si>
+  <si>
+    <t>Foreign Key References AdminID</t>
   </si>
 </sst>
 </file>
@@ -686,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{423C33E5-2E8B-4D17-8720-2B38F06ABDF5}">
-  <dimension ref="B2:D75"/>
+  <dimension ref="B2:D76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71:D75"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,182 +1122,193 @@
       </c>
       <c r="D54" s="3"/>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="4" t="s">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B55" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C56" s="2"/>
-      <c r="D56" s="3"/>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B57" s="1"/>
       <c r="C57" s="2"/>
       <c r="D57" s="3"/>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="B58" s="1"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="3"/>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D59" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D60" s="3"/>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>52</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D61" s="3"/>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D63" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D64" s="3"/>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>68</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="D65" s="3"/>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D66" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D67" s="3"/>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D68" s="3"/>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D69" s="3"/>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B71" s="4" t="s">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D70" s="3"/>
+    </row>
+    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C71" s="2"/>
-      <c r="D71" s="3"/>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B72" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D72" s="3" t="s">
-        <v>55</v>
-      </c>
+      <c r="C72" s="2"/>
+      <c r="D72" s="3"/>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B73" s="1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C76" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D75" s="3"/>
+      <c r="D76" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>